<commit_message>
ke: sch sth SPPM updated form
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Kenya/ke_sch_sth_sppm_202403_2_kk.xlsx
+++ b/SCH-STH/Impact assessments/Kenya/ke_sch_sth_sppm_202403_2_kk.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bonhe\Repositories\dsa-forms\SCH-STH\Impact assessments\Kenya\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Kenya\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{135D2F56-2481-4E6C-8634-4D041AC164C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C12412-3F01-4995-B8F8-3A5117A33094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="111">
   <si>
     <t>type</t>
   </si>
@@ -84,18 +84,9 @@
     <t>Stool Sample</t>
   </si>
   <si>
-    <t>barcode</t>
-  </si>
-  <si>
     <t>integer</t>
   </si>
   <si>
-    <t>. &gt; 400000 and . &lt; 500000</t>
-  </si>
-  <si>
-    <t>Re_enter_Child_ID</t>
-  </si>
-  <si>
     <t>begin_group</t>
   </si>
   <si>
@@ -231,12 +222,6 @@
     <t>English</t>
   </si>
   <si>
-    <t>(2024 Mar) - 2. SCH/STH – Stools</t>
-  </si>
-  <si>
-    <t>ke_sch_sth_sppm_202403_2_kk</t>
-  </si>
-  <si>
     <t>label::English</t>
   </si>
   <si>
@@ -282,54 +267,12 @@
     <t>allok_choice_duplicates</t>
   </si>
   <si>
-    <t>ke_k_202403</t>
-  </si>
-  <si>
     <t>calculate</t>
   </si>
   <si>
     <t>C1</t>
   </si>
   <si>
-    <t>select_one id_type</t>
-  </si>
-  <si>
-    <t>Will you scann the barcode or enter the code manualy</t>
-  </si>
-  <si>
-    <t>Child_ID_Survey_Barcode</t>
-  </si>
-  <si>
-    <t>Child ID Survey Barcode</t>
-  </si>
-  <si>
-    <t>regex(., '^(400000|4[0-9]{5}|500000)$')</t>
-  </si>
-  <si>
-    <t>Remove response, swipe forward to enter manually</t>
-  </si>
-  <si>
-    <t>Child_ID_Enter</t>
-  </si>
-  <si>
-    <t>Child ID Enter</t>
-  </si>
-  <si>
-    <t>6 Digits</t>
-  </si>
-  <si>
-    <t>Re enter Child ID</t>
-  </si>
-  <si>
-    <t>Enter exact as previous</t>
-  </si>
-  <si>
-    <t>. = ${Child_ID_Enter}</t>
-  </si>
-  <si>
-    <t>ID MUST be same as previous one</t>
-  </si>
-  <si>
     <t>C2</t>
   </si>
   <si>
@@ -351,30 +294,12 @@
     <t>join(' ', ${k_code_id})</t>
   </si>
   <si>
-    <t>k_id_type</t>
-  </si>
-  <si>
-    <t>${k_id_type} = 'Scanner'</t>
-  </si>
-  <si>
-    <t>${k_id_type} != 'Scanner'</t>
-  </si>
-  <si>
-    <t>k_code_id_calculate</t>
-  </si>
-  <si>
-    <t>if(${k_id_type} = 'Scanner', concat(${Child_ID_Survey_Barcode}) ,concat(${Child_ID_Enter}))</t>
-  </si>
-  <si>
     <t>if (${C2} = 1,'',substring-after(${C1},${k_code_id}))</t>
   </si>
   <si>
     <t>k_code_id</t>
   </si>
   <si>
-    <t>concat(${k_code_id_calculate})</t>
-  </si>
-  <si>
     <t>id_type</t>
   </si>
   <si>
@@ -414,9 +339,6 @@
     <t>no</t>
   </si>
   <si>
-    <t>Out of range! Must be between 400000 and 500000</t>
-  </si>
-  <si>
     <t>${k_Team_Number} = 'other'</t>
   </si>
   <si>
@@ -424,6 +346,15 @@
   </si>
   <si>
     <t>read_only</t>
+  </si>
+  <si>
+    <t>(2024 Mar) - 2. SCH/STH – Stools V1.1</t>
+  </si>
+  <si>
+    <t>ke_sch_sth_sppm_202403_2_kk_v1_1</t>
+  </si>
+  <si>
+    <t>ke_k_202403_v1_1</t>
   </si>
 </sst>
 </file>
@@ -848,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="A12" activeCellId="1" sqref="A11:XFD11 A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,10 +808,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>6</v>
@@ -889,13 +820,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>2</v>
@@ -907,7 +838,7 @@
         <v>7</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -915,7 +846,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>11</v>
@@ -927,23 +858,23 @@
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>12</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -951,16 +882,16 @@
         <v>13</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -968,13 +899,13 @@
         <v>13</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>15</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -982,13 +913,13 @@
         <v>13</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -996,38 +927,38 @@
         <v>13</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>84</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>17</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1035,7 +966,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>19</v>
@@ -1047,401 +978,278 @@
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
     </row>
-    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>89</v>
-      </c>
-      <c r="B11" t="s">
-        <v>109</v>
-      </c>
-      <c r="C11" s="7" t="s">
+    <row r="11" spans="1:13" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="I11" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="I12" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
-      <c r="G11"/>
-      <c r="H11"/>
-      <c r="I11"/>
-      <c r="J11" t="s">
-        <v>59</v>
-      </c>
-      <c r="K11"/>
-      <c r="L11"/>
-    </row>
-    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" t="s">
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
         <v>91</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="J12" t="s">
-        <v>129</v>
-      </c>
-      <c r="K12"/>
-      <c r="L12"/>
-    </row>
-    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>95</v>
-      </c>
       <c r="C13" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="J13" t="s">
-        <v>59</v>
+        <v>86</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="K13"/>
       <c r="L13"/>
     </row>
-    <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C15" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="F14" s="7" t="s">
+      <c r="B21" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="J14" t="s">
-        <v>59</v>
-      </c>
-      <c r="K14"/>
-      <c r="L14"/>
-    </row>
-    <row r="15" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>87</v>
-      </c>
-      <c r="B15" t="s">
-        <v>112</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="J15"/>
-      <c r="K15"/>
-      <c r="L15"/>
-    </row>
-    <row r="16" spans="1:13" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="C16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="I16" s="11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="C17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="I17" s="12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" t="s">
-        <v>115</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="K18"/>
-      <c r="L18"/>
-      <c r="M18" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="J21" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J22" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>29</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>30</v>
       </c>
+      <c r="H23" s="7" t="s">
+        <v>95</v>
+      </c>
       <c r="J23" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>64</v>
+        <v>101</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>64</v>
+        <v>31</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>95</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="J26" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="L25" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="J28" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="J29" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="J30" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="L30" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>128</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1465,13 +1273,13 @@
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>15</v>
@@ -1479,156 +1287,156 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="B17" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
       <c r="C17" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="B18" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="C18" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1641,7 +1449,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1653,30 +1461,30 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>69</v>
+        <v>108</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>70</v>
+        <v>109</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>